<commit_message>
Client included in single and Bulk order
Client included in single and Bulk order


(cherry picked from commit 30150268904f5f58ee900fc8fa9b2011f8acbfba)

Co-authored-by: mani0807 <Manikandan.V@stellaripl.com>
</commit_message>
<xml_diff>
--- a/public/template/Accurate_sample_template.xlsx
+++ b/public/template/Accurate_sample_template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Developer\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\stellar-oms(dev)\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A07888-2C4C-4FE1-A3B5-BE4B9A55D330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD258004-F812-44E2-95E5-B90A2C73DBF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>Order Received Data and Time</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>Search &amp; Typing</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Accurate</t>
   </si>
 </sst>
 </file>
@@ -111,7 +117,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,6 +254,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -615,11 +628,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -975,10 +989,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -987,11 +1001,12 @@
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="36.33203125" customWidth="1"/>
     <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="9" width="16" customWidth="1"/>
-    <col min="12" max="12" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" customWidth="1"/>
+    <col min="8" max="10" width="16" customWidth="1"/>
+    <col min="13" max="13" width="10.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1005,31 +1020,34 @@
         <v>3</v>
       </c>
       <c r="E1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>45436.041666666664</v>
       </c>
@@ -1042,32 +1060,35 @@
       <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>45439.083333333336</v>
       </c>
@@ -1080,28 +1101,31 @@
       <c r="D3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added New client for testing-gangaraj
Added New client for testing-gangaraj
</commit_message>
<xml_diff>
--- a/public/template/Accurate_sample_template.xlsx
+++ b/public/template/Accurate_sample_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\stellar-oms(dev)\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD258004-F812-44E2-95E5-B90A2C73DBF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45775D8A-4DDD-4814-9CA5-A15A51DC8935}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -633,7 +633,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -992,7 +992,7 @@
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>